<commit_message>
add pp 1.0.2 test
</commit_message>
<xml_diff>
--- a/apps.xlsx
+++ b/apps.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="18">
   <si>
     <t>app_name</t>
   </si>
@@ -34,13 +34,19 @@
     <t>build</t>
   </si>
   <si>
+    <t>PautangPeso(test)</t>
+  </si>
+  <si>
+    <t>ph.lhl.pautangpeso</t>
+  </si>
+  <si>
+    <t>1.0.2</t>
+  </si>
+  <si>
+    <t>https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso1.0.2_2_test.ipa</t>
+  </si>
+  <si>
     <t>PautangPeso</t>
-  </si>
-  <si>
-    <t>ph.lhl.pautangpeso</t>
-  </si>
-  <si>
-    <t>1.0.2</t>
   </si>
   <si>
     <t>https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso1.0.22.ipa</t>
@@ -72,10 +78,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -97,14 +103,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -118,8 +116,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -133,8 +140,82 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -142,22 +223,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -165,66 +230,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -245,31 +251,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -281,145 +323,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -430,6 +436,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -448,11 +463,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -474,24 +495,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -513,11 +521,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -535,142 +541,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1009,13 +1015,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="4" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="5" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="24.2109375" customWidth="1"/>
     <col min="2" max="2" width="22.7890625" customWidth="1"/>
@@ -1059,7 +1065,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -1068,24 +1074,24 @@
         <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -1093,10 +1099,10 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
@@ -1105,15 +1111,33 @@
         <v>15</v>
       </c>
       <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.1.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.1.ipa"/>
-    <hyperlink ref="D4" r:id="rId2" display="https://iosinhouse.tangbull.com/ipesoIosAdhoc/Ipeso.ipa"/>
-    <hyperlink ref="D3" r:id="rId3" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.2.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.2.ipa"/>
-    <hyperlink ref="D2" r:id="rId4" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso1.0.22.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso1.0.22.ipa"/>
+    <hyperlink ref="D6" r:id="rId1" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.1.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.1.ipa"/>
+    <hyperlink ref="D5" r:id="rId2" display="https://iosinhouse.tangbull.com/ipesoIosAdhoc/Ipeso.ipa"/>
+    <hyperlink ref="D4" r:id="rId3" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.2.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.2.ipa"/>
+    <hyperlink ref="D3" r:id="rId4" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso1.0.22.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso1.0.22.ipa"/>
+    <hyperlink ref="D2" r:id="rId5" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso1.0.2_2_test.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso1.0.2_2_test.ipa"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
add ip new test
</commit_message>
<xml_diff>
--- a/apps.xlsx
+++ b/apps.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="16">
   <si>
     <t>app_name</t>
   </si>
@@ -40,6 +40,12 @@
     <t>com.linkcredited.ipeso</t>
   </si>
   <si>
+    <t>1.0.2</t>
+  </si>
+  <si>
+    <t>https://bitbucket.org/cop-dev/ios-apps/downloads/Ipeso-1.0.2-2-test.ipa</t>
+  </si>
+  <si>
     <t>1.0.1</t>
   </si>
   <si>
@@ -50,9 +56,6 @@
   </si>
   <si>
     <t>ph.lhl.pautangpeso</t>
-  </si>
-  <si>
-    <t>1.0.2</t>
   </si>
   <si>
     <t>https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.2-4.ipa</t>
@@ -69,9 +72,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="20">
@@ -99,6 +102,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -106,16 +117,70 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -130,7 +195,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -145,83 +210,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -236,19 +239,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -260,163 +407,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -454,11 +457,28 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -478,17 +498,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -498,17 +512,6 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -532,142 +535,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1006,13 +1009,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="3" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="4" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="24.2109375" customWidth="1"/>
     <col min="2" max="2" width="22.7890625" customWidth="1"/>
@@ -1056,43 +1059,61 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="E3">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="E4">
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.2-3.ipa"/>
-    <hyperlink ref="D3" r:id="rId2" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.2-4.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.2-4.ipa"/>
-    <hyperlink ref="D2" r:id="rId3" display="https://bitbucket.org/cop-dev/ios-apps/downloads/Ipeso-1.0.1-test1.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/Ipeso-1.0.1-test1.ipa"/>
+    <hyperlink ref="D5" r:id="rId1" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.2-3.ipa"/>
+    <hyperlink ref="D4" r:id="rId2" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.2-4.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.2-4.ipa"/>
+    <hyperlink ref="D3" r:id="rId3" display="https://bitbucket.org/cop-dev/ios-apps/downloads/Ipeso-1.0.1-test1.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/Ipeso-1.0.1-test1.ipa"/>
+    <hyperlink ref="D2" r:id="rId4" display="https://bitbucket.org/cop-dev/ios-apps/downloads/Ipeso-1.0.2-2-test.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/Ipeso-1.0.2-2-test.ipa"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
add cashwill prod 1.0.1
</commit_message>
<xml_diff>
--- a/apps.xlsx
+++ b/apps.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16860"/>
+    <workbookView windowHeight="15200"/>
   </bookViews>
   <sheets>
     <sheet name="Philippines" sheetId="1" r:id="rId1"/>
@@ -40,15 +40,18 @@
     <t>ph.euiwr.cashwill</t>
   </si>
   <si>
+    <t>1.0.1</t>
+  </si>
+  <si>
+    <t>https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.1-1-prod.ipa</t>
+  </si>
+  <si>
+    <t>Cashwill(test)</t>
+  </si>
+  <si>
     <t>1.0.0</t>
   </si>
   <si>
-    <t>https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.0-3-prod.ipa</t>
-  </si>
-  <si>
-    <t>Cashwill(test)</t>
-  </si>
-  <si>
     <t>https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.0-2.test.ipa</t>
   </si>
   <si>
@@ -104,9 +107,6 @@
   </si>
   <si>
     <t>https://bitbucket.org/cop-dev/ios-apps/downloads/Ipeso-1.0.2-2-test.ipa</t>
-  </si>
-  <si>
-    <t>1.0.1</t>
   </si>
   <si>
     <t>https://bitbucket.org/cop-dev/ios-apps/downloads/Ipeso-1.0.1-test1.ipa</t>
@@ -124,8 +124,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
@@ -154,14 +154,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -170,81 +162,69 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -259,7 +239,28 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -273,9 +274,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -290,19 +290,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -314,49 +434,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -368,109 +470,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -481,6 +481,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -503,27 +512,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -539,21 +543,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -575,6 +564,17 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -586,118 +586,118 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -706,22 +706,22 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1063,7 +1063,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="4"/>
@@ -1105,7 +1105,7 @@
         <v>8</v>
       </c>
       <c r="E2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1116,10 +1116,10 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -1127,16 +1127,16 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -1144,16 +1144,16 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -1161,16 +1161,16 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E6">
         <v>3</v>
@@ -1178,16 +1178,16 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E7">
         <v>2</v>
@@ -1195,16 +1195,16 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -1212,13 +1212,13 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>30</v>
@@ -1229,13 +1229,13 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>31</v>
@@ -1246,13 +1246,13 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>32</v>
@@ -1272,7 +1272,7 @@
     <hyperlink ref="D5" r:id="rId7" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pesoq-test-1.5.6-3.ipa"/>
     <hyperlink ref="D4" r:id="rId8" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pesocash-test-1.3.0-1.ipa"/>
     <hyperlink ref="D3" r:id="rId9" display="https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.0-2.test.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.0-2.test.ipa"/>
-    <hyperlink ref="D2" r:id="rId10" display="https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.0-3-prod.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.0-3-prod.ipa"/>
+    <hyperlink ref="D2" r:id="rId10" display="https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.1-1-prod.ipa"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
add cashwill test 1.0.2
</commit_message>
<xml_diff>
--- a/apps.xlsx
+++ b/apps.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="34">
   <si>
     <t>app_name</t>
   </si>
@@ -34,21 +34,27 @@
     <t>build</t>
   </si>
   <si>
+    <t>Cashwill(test)</t>
+  </si>
+  <si>
+    <t>ph.euiwr.cashwill</t>
+  </si>
+  <si>
+    <t>1.0.2</t>
+  </si>
+  <si>
+    <t>https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.2-1-test.ipa</t>
+  </si>
+  <si>
     <t>Cashwill(prod)</t>
   </si>
   <si>
-    <t>ph.euiwr.cashwill</t>
-  </si>
-  <si>
     <t>1.0.1</t>
   </si>
   <si>
     <t>https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.1-1-prod.ipa</t>
   </si>
   <si>
-    <t>Cashwill(test)</t>
-  </si>
-  <si>
     <t>1.0.0</t>
   </si>
   <si>
@@ -101,9 +107,6 @@
   </si>
   <si>
     <t>com.linkcredited.ipeso</t>
-  </si>
-  <si>
-    <t>1.0.2</t>
   </si>
   <si>
     <t>https://bitbucket.org/cop-dev/ios-apps/downloads/Ipeso-1.0.2-2-test.ipa</t>
@@ -125,8 +128,8 @@
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -148,6 +151,20 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -162,67 +179,20 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -238,20 +208,46 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -260,22 +256,29 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -290,25 +293,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -320,157 +473,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -489,21 +492,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -532,17 +520,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -573,6 +561,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -586,142 +589,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1060,10 +1063,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="4"/>
@@ -1122,38 +1125,38 @@
         <v>11</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="E4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -1161,36 +1164,36 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
         <v>20</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="E6">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
         <v>24</v>
       </c>
-      <c r="B7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>25</v>
       </c>
       <c r="E7">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1198,24 +1201,24 @@
         <v>26</v>
       </c>
       <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="E8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -1229,50 +1232,68 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E10">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>32</v>
       </c>
       <c r="E11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D11" r:id="rId1" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.2-3.ipa"/>
-    <hyperlink ref="D10" r:id="rId2" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.2-4.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.2-4.ipa"/>
-    <hyperlink ref="D9" r:id="rId3" display="https://bitbucket.org/cop-dev/ios-apps/downloads/Ipeso-1.0.1-test1.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/Ipeso-1.0.1-test1.ipa"/>
-    <hyperlink ref="D8" r:id="rId4" display="https://bitbucket.org/cop-dev/ios-apps/downloads/Ipeso-1.0.2-2-test.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/Ipeso-1.0.2-2-test.ipa"/>
-    <hyperlink ref="D7" r:id="rId5" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.3-2-test.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.3-2-test.ipa"/>
-    <hyperlink ref="D6" r:id="rId6" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.3-3-prod.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.3-3-prod.ipa"/>
-    <hyperlink ref="D5" r:id="rId7" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pesoq-test-1.5.6-3.ipa"/>
-    <hyperlink ref="D4" r:id="rId8" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pesocash-test-1.3.0-1.ipa"/>
-    <hyperlink ref="D3" r:id="rId9" display="https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.0-2.test.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.0-2.test.ipa"/>
-    <hyperlink ref="D2" r:id="rId10" display="https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.1-1-prod.ipa"/>
+    <hyperlink ref="D12" r:id="rId1" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.2-3.ipa"/>
+    <hyperlink ref="D11" r:id="rId2" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.2-4.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.2-4.ipa"/>
+    <hyperlink ref="D10" r:id="rId3" display="https://bitbucket.org/cop-dev/ios-apps/downloads/Ipeso-1.0.1-test1.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/Ipeso-1.0.1-test1.ipa"/>
+    <hyperlink ref="D9" r:id="rId4" display="https://bitbucket.org/cop-dev/ios-apps/downloads/Ipeso-1.0.2-2-test.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/Ipeso-1.0.2-2-test.ipa"/>
+    <hyperlink ref="D8" r:id="rId5" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.3-2-test.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.3-2-test.ipa"/>
+    <hyperlink ref="D7" r:id="rId6" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.3-3-prod.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.3-3-prod.ipa"/>
+    <hyperlink ref="D6" r:id="rId7" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pesoq-test-1.5.6-3.ipa"/>
+    <hyperlink ref="D5" r:id="rId8" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pesocash-test-1.3.0-1.ipa"/>
+    <hyperlink ref="D4" r:id="rId9" display="https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.0-2.test.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.0-2.test.ipa"/>
+    <hyperlink ref="D3" r:id="rId10" display="https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.1-1-prod.ipa"/>
+    <hyperlink ref="D2" r:id="rId11" display="https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.2-1-test.ipa"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
add cashwill prod 1.0.2
</commit_message>
<xml_diff>
--- a/apps.xlsx
+++ b/apps.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="35">
   <si>
     <t>app_name</t>
   </si>
@@ -34,19 +34,22 @@
     <t>build</t>
   </si>
   <si>
+    <t>Cashwill(prod)</t>
+  </si>
+  <si>
+    <t>ph.euiwr.cashwill</t>
+  </si>
+  <si>
+    <t>1.0.2</t>
+  </si>
+  <si>
+    <t>https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.2-1-prod.ipa</t>
+  </si>
+  <si>
     <t>Cashwill(test)</t>
   </si>
   <si>
-    <t>ph.euiwr.cashwill</t>
-  </si>
-  <si>
-    <t>1.0.2</t>
-  </si>
-  <si>
     <t>https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.2-1-test.ipa</t>
-  </si>
-  <si>
-    <t>Cashwill(prod)</t>
   </si>
   <si>
     <t>1.0.1</t>
@@ -126,10 +129,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -156,15 +159,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -178,10 +190,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -194,91 +207,81 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -293,31 +296,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -329,151 +464,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -484,24 +487,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -520,42 +505,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -576,6 +529,36 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -584,147 +567,167 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1063,7 +1066,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -1119,10 +1122,10 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1136,44 +1139,44 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="E4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="E5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -1181,64 +1184,64 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="E7">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="E8">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="E9">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>31</v>
@@ -1249,51 +1252,69 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E11">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D12" r:id="rId1" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.2-3.ipa"/>
-    <hyperlink ref="D11" r:id="rId2" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.2-4.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.2-4.ipa"/>
-    <hyperlink ref="D10" r:id="rId3" display="https://bitbucket.org/cop-dev/ios-apps/downloads/Ipeso-1.0.1-test1.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/Ipeso-1.0.1-test1.ipa"/>
-    <hyperlink ref="D9" r:id="rId4" display="https://bitbucket.org/cop-dev/ios-apps/downloads/Ipeso-1.0.2-2-test.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/Ipeso-1.0.2-2-test.ipa"/>
-    <hyperlink ref="D8" r:id="rId5" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.3-2-test.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.3-2-test.ipa"/>
-    <hyperlink ref="D7" r:id="rId6" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.3-3-prod.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.3-3-prod.ipa"/>
-    <hyperlink ref="D6" r:id="rId7" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pesoq-test-1.5.6-3.ipa"/>
-    <hyperlink ref="D5" r:id="rId8" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pesocash-test-1.3.0-1.ipa"/>
-    <hyperlink ref="D4" r:id="rId9" display="https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.0-2.test.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.0-2.test.ipa"/>
-    <hyperlink ref="D3" r:id="rId10" display="https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.1-1-prod.ipa"/>
-    <hyperlink ref="D2" r:id="rId11" display="https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.2-1-test.ipa"/>
+    <hyperlink ref="D13" r:id="rId1" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.2-3.ipa"/>
+    <hyperlink ref="D12" r:id="rId2" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.2-4.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.2-4.ipa"/>
+    <hyperlink ref="D11" r:id="rId3" display="https://bitbucket.org/cop-dev/ios-apps/downloads/Ipeso-1.0.1-test1.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/Ipeso-1.0.1-test1.ipa"/>
+    <hyperlink ref="D10" r:id="rId4" display="https://bitbucket.org/cop-dev/ios-apps/downloads/Ipeso-1.0.2-2-test.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/Ipeso-1.0.2-2-test.ipa"/>
+    <hyperlink ref="D9" r:id="rId5" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.3-2-test.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.3-2-test.ipa"/>
+    <hyperlink ref="D8" r:id="rId6" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.3-3-prod.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.3-3-prod.ipa"/>
+    <hyperlink ref="D7" r:id="rId7" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pesoq-test-1.5.6-3.ipa"/>
+    <hyperlink ref="D6" r:id="rId8" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pesocash-test-1.3.0-1.ipa"/>
+    <hyperlink ref="D5" r:id="rId9" display="https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.0-2.test.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.0-2.test.ipa"/>
+    <hyperlink ref="D4" r:id="rId10" display="https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.1-1-prod.ipa"/>
+    <hyperlink ref="D3" r:id="rId11" display="https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.2-1-test.ipa"/>
+    <hyperlink ref="D2" r:id="rId12" display="https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.2-1-prod.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.2-1-prod.ipa"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
pq pro test add
</commit_message>
<xml_diff>
--- a/apps.xlsx
+++ b/apps.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="55">
   <si>
     <t>app_name</t>
   </si>
@@ -34,19 +34,22 @@
     <t>build</t>
   </si>
   <si>
+    <t>PesoQ Pro(test)</t>
+  </si>
+  <si>
+    <t>com.loan.pesoqpro</t>
+  </si>
+  <si>
+    <t>1.0.1</t>
+  </si>
+  <si>
+    <t>https://bitbucket.org/zhufine/iosfine/downloads/pesoq-pro-test-1.0.1-3.ipa</t>
+  </si>
+  <si>
     <t>PesoQ Pro</t>
   </si>
   <si>
-    <t>com.loan.pesoqpro</t>
-  </si>
-  <si>
-    <t>1.0.1</t>
-  </si>
-  <si>
     <t>https://bitbucket.org/zhufine/iosfine/downloads/pesoq-pro-1.0.1-1-prod.ipa</t>
-  </si>
-  <si>
-    <t>PesoQ Pro(test)</t>
   </si>
   <si>
     <t>https://bitbucket.org/zhufine/iosfine/downloads/pesoq-pro-test-1.0.1-1.ipa</t>
@@ -186,9 +189,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
@@ -217,14 +220,60 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -238,8 +287,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -254,37 +311,6 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -292,14 +318,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
@@ -309,14 +327,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -331,13 +341,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -353,55 +356,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -413,127 +536,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -544,6 +547,41 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -586,32 +624,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -635,156 +647,147 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1123,7 +1126,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -1168,7 +1171,7 @@
         <v>8</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1190,67 +1193,67 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>13</v>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="E4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>15</v>
+      <c r="D5" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="E6">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="E7">
         <v>3</v>
@@ -1258,67 +1261,67 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="E8">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="E9">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="E10">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="B11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -1326,16 +1329,16 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="B12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -1343,13 +1346,13 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>37</v>
@@ -1360,47 +1363,47 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="E14">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B15" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="E15">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>44</v>
@@ -1411,64 +1414,64 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="E17">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E18">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B19" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="E19">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C20" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>51</v>
@@ -1479,61 +1482,79 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="C21" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>52</v>
       </c>
       <c r="E21">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
         <v>24</v>
       </c>
-      <c r="C22" t="s">
-        <v>33</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E22">
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E23">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D22" r:id="rId1" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.2-3.ipa"/>
-    <hyperlink ref="D21" r:id="rId2" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.2-4.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.2-4.ipa"/>
-    <hyperlink ref="D20" r:id="rId3" display="https://bitbucket.org/cop-dev/ios-apps/downloads/Ipeso-1.0.1-test1.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/Ipeso-1.0.1-test1.ipa"/>
-    <hyperlink ref="D19" r:id="rId4" display="https://bitbucket.org/cop-dev/ios-apps/downloads/Ipeso-1.0.2-2-test.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/Ipeso-1.0.2-2-test.ipa"/>
-    <hyperlink ref="D18" r:id="rId5" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.3-2-test.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.3-2-test.ipa"/>
-    <hyperlink ref="D17" r:id="rId6" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.3-3-prod.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.3-3-prod.ipa"/>
-    <hyperlink ref="D16" r:id="rId7" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pesoq-test-1.5.6-3.ipa"/>
-    <hyperlink ref="D15" r:id="rId8" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pesocash-test-1.3.0-1.ipa"/>
-    <hyperlink ref="D14" r:id="rId9" display="https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.0-2.test.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.0-2.test.ipa"/>
-    <hyperlink ref="D13" r:id="rId10" display="https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.1-1-prod.ipa"/>
-    <hyperlink ref="D12" r:id="rId11" display="https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.2-1-test.ipa"/>
-    <hyperlink ref="D11" r:id="rId12" display="https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.2-1-prod.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.2-1-prod.ipa"/>
-    <hyperlink ref="D10" r:id="rId13" display="https://bitbucket.org/ios4/ios/downloads/pautangpeso-1.0.4-1-test.ipa"/>
-    <hyperlink ref="D9" r:id="rId14" display="https://bitbucket.org/ios4/ios/downloads/pesoq-1.5.6-3-prod.ipa" tooltip="https://bitbucket.org/ios4/ios/downloads/pesoq-1.5.6-3-prod.ipa"/>
-    <hyperlink ref="D8" r:id="rId15" display="https://bitbucket.org/ios4/ios/downloads/pautangpeso-1.0.4-1-prod.ipa"/>
-    <hyperlink ref="D7" r:id="rId16" display="https://bitbucket.org/ios4/ios/downloads/pesoq-1.5.6-3-test.ipa"/>
-    <hyperlink ref="D6" r:id="rId17" display="https://bitbucket.org/ios4/ios/downloads/pesoq-prod-1.5.7-1.ipa" tooltip="https://bitbucket.org/ios4/ios/downloads/pesoq-prod-1.5.7-1.ipa"/>
-    <hyperlink ref="D5" r:id="rId18" display="https://bitbucket.org/ios4/ios/downloads/ipesovip-test-1.0.1-1.ipa"/>
-    <hyperlink ref="D4" r:id="rId19" display="https://bitbucket.org/zhufine/iosfine/downloads/ipesovip-prod-1.0.1-2.ipa" tooltip="https://bitbucket.org/zhufine/iosfine/downloads/ipesovip-prod-1.0.1-2.ipa"/>
-    <hyperlink ref="D3" r:id="rId20" display="https://bitbucket.org/zhufine/iosfine/downloads/pesoq-pro-test-1.0.1-1.ipa" tooltip="https://bitbucket.org/zhufine/iosfine/downloads/pesoq-pro-test-1.0.1-1.ipa"/>
-    <hyperlink ref="D2" r:id="rId21" display="https://bitbucket.org/zhufine/iosfine/downloads/pesoq-pro-1.0.1-1-prod.ipa" tooltip="https://bitbucket.org/zhufine/iosfine/downloads/pesoq-pro-1.0.1-1-prod.ipa"/>
+    <hyperlink ref="D23" r:id="rId1" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.2-3.ipa"/>
+    <hyperlink ref="D22" r:id="rId2" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.2-4.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.2-4.ipa"/>
+    <hyperlink ref="D21" r:id="rId3" display="https://bitbucket.org/cop-dev/ios-apps/downloads/Ipeso-1.0.1-test1.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/Ipeso-1.0.1-test1.ipa"/>
+    <hyperlink ref="D20" r:id="rId4" display="https://bitbucket.org/cop-dev/ios-apps/downloads/Ipeso-1.0.2-2-test.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/Ipeso-1.0.2-2-test.ipa"/>
+    <hyperlink ref="D19" r:id="rId5" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.3-2-test.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.3-2-test.ipa"/>
+    <hyperlink ref="D18" r:id="rId6" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.3-3-prod.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.3-3-prod.ipa"/>
+    <hyperlink ref="D17" r:id="rId7" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pesoq-test-1.5.6-3.ipa"/>
+    <hyperlink ref="D16" r:id="rId8" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pesocash-test-1.3.0-1.ipa"/>
+    <hyperlink ref="D15" r:id="rId9" display="https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.0-2.test.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.0-2.test.ipa"/>
+    <hyperlink ref="D14" r:id="rId10" display="https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.1-1-prod.ipa"/>
+    <hyperlink ref="D13" r:id="rId11" display="https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.2-1-test.ipa"/>
+    <hyperlink ref="D12" r:id="rId12" display="https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.2-1-prod.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.2-1-prod.ipa"/>
+    <hyperlink ref="D11" r:id="rId13" display="https://bitbucket.org/ios4/ios/downloads/pautangpeso-1.0.4-1-test.ipa"/>
+    <hyperlink ref="D10" r:id="rId14" display="https://bitbucket.org/ios4/ios/downloads/pesoq-1.5.6-3-prod.ipa" tooltip="https://bitbucket.org/ios4/ios/downloads/pesoq-1.5.6-3-prod.ipa"/>
+    <hyperlink ref="D9" r:id="rId15" display="https://bitbucket.org/ios4/ios/downloads/pautangpeso-1.0.4-1-prod.ipa"/>
+    <hyperlink ref="D8" r:id="rId16" display="https://bitbucket.org/ios4/ios/downloads/pesoq-1.5.6-3-test.ipa"/>
+    <hyperlink ref="D7" r:id="rId17" display="https://bitbucket.org/ios4/ios/downloads/pesoq-prod-1.5.7-1.ipa" tooltip="https://bitbucket.org/ios4/ios/downloads/pesoq-prod-1.5.7-1.ipa"/>
+    <hyperlink ref="D6" r:id="rId18" display="https://bitbucket.org/ios4/ios/downloads/ipesovip-test-1.0.1-1.ipa"/>
+    <hyperlink ref="D5" r:id="rId19" display="https://bitbucket.org/zhufine/iosfine/downloads/ipesovip-prod-1.0.1-2.ipa" tooltip="https://bitbucket.org/zhufine/iosfine/downloads/ipesovip-prod-1.0.1-2.ipa"/>
+    <hyperlink ref="D4" r:id="rId20" display="https://bitbucket.org/zhufine/iosfine/downloads/pesoq-pro-test-1.0.1-1.ipa" tooltip="https://bitbucket.org/zhufine/iosfine/downloads/pesoq-pro-test-1.0.1-1.ipa"/>
+    <hyperlink ref="D3" r:id="rId21" display="https://bitbucket.org/zhufine/iosfine/downloads/pesoq-pro-1.0.1-1-prod.ipa" tooltip="https://bitbucket.org/zhufine/iosfine/downloads/pesoq-pro-1.0.1-1-prod.ipa"/>
+    <hyperlink ref="D2" r:id="rId22" display="https://bitbucket.org/zhufine/iosfine/downloads/pesoq-pro-test-1.0.1-3.ipa"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
add prod ipeso vip
</commit_message>
<xml_diff>
--- a/apps.xlsx
+++ b/apps.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="64">
   <si>
     <t>app_name</t>
   </si>
@@ -34,15 +34,21 @@
     <t>build</t>
   </si>
   <si>
+    <t>IPeso VIP</t>
+  </si>
+  <si>
+    <t>com.linkcredited.ipesovip</t>
+  </si>
+  <si>
+    <t>1.0.2</t>
+  </si>
+  <si>
+    <t>https://bitbucket.org/zhufine/iosapp/downloads/ipesovip-1.0.2-1-prod.ipa</t>
+  </si>
+  <si>
     <t>IPeso VIP(test)</t>
   </si>
   <si>
-    <t>com.linkcredited.ipesovip</t>
-  </si>
-  <si>
-    <t>1.0.2</t>
-  </si>
-  <si>
     <t>https://bitbucket.org/zhufine/iosapp/downloads/ipesovip-1.0.2-1-test.ipa</t>
   </si>
   <si>
@@ -89,9 +95,6 @@
   </si>
   <si>
     <t>https://bitbucket.org/zhufine/iosfine/downloads/pesoq-pro-test-1.0.1-1.ipa</t>
-  </si>
-  <si>
-    <t>IPeso VIP</t>
   </si>
   <si>
     <t>https://bitbucket.org/zhufine/iosfine/downloads/ipesovip-prod-1.0.1-2.ipa</t>
@@ -214,9 +217,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -250,6 +253,81 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -258,16 +336,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -275,36 +346,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -319,28 +360,6 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -348,28 +367,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -386,13 +389,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -404,13 +497,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -422,7 +509,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -434,19 +527,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -458,109 +557,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -574,26 +577,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -617,7 +611,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -625,19 +619,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -657,17 +655,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -676,139 +679,139 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1150,10 +1153,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="4"/>
@@ -1195,123 +1198,123 @@
         <v>8</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E3">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E4">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="E5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E7">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>20</v>
+      <c r="D9" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -1319,50 +1322,50 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E10">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -1370,19 +1373,19 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>25</v>
       </c>
       <c r="E13">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1393,44 +1396,44 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="E15">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="B16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="E16">
         <v>3</v>
@@ -1438,67 +1441,67 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="E17">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B18" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="E18">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B19" t="s">
-        <v>35</v>
-      </c>
-      <c r="C19" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="E19">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B20" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -1506,16 +1509,16 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C21" t="s">
         <v>7</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -1523,13 +1526,13 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C22" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>47</v>
@@ -1540,47 +1543,47 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="E23">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B24" t="s">
-        <v>51</v>
-      </c>
-      <c r="C24" t="s">
-        <v>52</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="E24">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="B25" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="C25" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>54</v>
@@ -1591,64 +1594,64 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>55</v>
       </c>
       <c r="E26">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C27" t="s">
-        <v>14</v>
-      </c>
-      <c r="D27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>56</v>
       </c>
       <c r="E27">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B28" t="s">
-        <v>58</v>
-      </c>
-      <c r="C28" t="s">
-        <v>7</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="E28">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B29" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C29" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>60</v>
@@ -1659,70 +1662,88 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="C30" t="s">
-        <v>7</v>
-      </c>
-      <c r="D30" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>61</v>
       </c>
       <c r="E30">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B31" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C31" t="s">
         <v>7</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D31" s="2" t="s">
         <v>62</v>
       </c>
       <c r="E31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E32">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D31" r:id="rId1" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.2-3.ipa"/>
-    <hyperlink ref="D30" r:id="rId2" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.2-4.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.2-4.ipa"/>
-    <hyperlink ref="D29" r:id="rId3" display="https://bitbucket.org/cop-dev/ios-apps/downloads/Ipeso-1.0.1-test1.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/Ipeso-1.0.1-test1.ipa"/>
-    <hyperlink ref="D28" r:id="rId4" display="https://bitbucket.org/cop-dev/ios-apps/downloads/Ipeso-1.0.2-2-test.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/Ipeso-1.0.2-2-test.ipa"/>
-    <hyperlink ref="D27" r:id="rId5" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.3-2-test.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.3-2-test.ipa"/>
-    <hyperlink ref="D26" r:id="rId6" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.3-3-prod.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.3-3-prod.ipa"/>
-    <hyperlink ref="D25" r:id="rId7" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pesoq-test-1.5.6-3.ipa"/>
-    <hyperlink ref="D24" r:id="rId8" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pesocash-test-1.3.0-1.ipa"/>
-    <hyperlink ref="D23" r:id="rId9" display="https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.0-2.test.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.0-2.test.ipa"/>
-    <hyperlink ref="D22" r:id="rId10" display="https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.1-1-prod.ipa"/>
-    <hyperlink ref="D21" r:id="rId11" display="https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.2-1-test.ipa"/>
-    <hyperlink ref="D20" r:id="rId12" display="https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.2-1-prod.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.2-1-prod.ipa"/>
-    <hyperlink ref="D19" r:id="rId13" display="https://bitbucket.org/ios4/ios/downloads/pautangpeso-1.0.4-1-test.ipa"/>
-    <hyperlink ref="D18" r:id="rId14" display="https://bitbucket.org/ios4/ios/downloads/pesoq-1.5.6-3-prod.ipa" tooltip="https://bitbucket.org/ios4/ios/downloads/pesoq-1.5.6-3-prod.ipa"/>
-    <hyperlink ref="D17" r:id="rId15" display="https://bitbucket.org/ios4/ios/downloads/pautangpeso-1.0.4-1-prod.ipa"/>
-    <hyperlink ref="D16" r:id="rId16" display="https://bitbucket.org/ios4/ios/downloads/pesoq-1.5.6-3-test.ipa"/>
-    <hyperlink ref="D15" r:id="rId17" display="https://bitbucket.org/ios4/ios/downloads/pesoq-prod-1.5.7-1.ipa" tooltip="https://bitbucket.org/ios4/ios/downloads/pesoq-prod-1.5.7-1.ipa"/>
-    <hyperlink ref="D14" r:id="rId18" display="https://bitbucket.org/ios4/ios/downloads/ipesovip-test-1.0.1-1.ipa"/>
-    <hyperlink ref="D13" r:id="rId19" display="https://bitbucket.org/zhufine/iosfine/downloads/ipesovip-prod-1.0.1-2.ipa" tooltip="https://bitbucket.org/zhufine/iosfine/downloads/ipesovip-prod-1.0.1-2.ipa"/>
-    <hyperlink ref="D12" r:id="rId20" display="https://bitbucket.org/zhufine/iosfine/downloads/pesoq-pro-test-1.0.1-1.ipa" tooltip="https://bitbucket.org/zhufine/iosfine/downloads/pesoq-pro-test-1.0.1-1.ipa"/>
-    <hyperlink ref="D11" r:id="rId21" display="https://bitbucket.org/zhufine/iosfine/downloads/pesoq-pro-1.0.1-1-prod.ipa" tooltip="https://bitbucket.org/zhufine/iosfine/downloads/pesoq-pro-1.0.1-1-prod.ipa"/>
-    <hyperlink ref="D10" r:id="rId22" display="https://bitbucket.org/zhufine/iosfine/downloads/pesoq-pro-test-1.0.1-3.ipa"/>
-    <hyperlink ref="D8" r:id="rId23" display="https://bitbucket.org/zhufine/iosfine/downloads/pesoq-pro-1.0.2-1-test.ipa"/>
-    <hyperlink ref="D9" r:id="rId24" display="https://bitbucket.org/zhufine/iosfine/downloads/pesoq-pro-1.0.2-1-prod.ipa"/>
-    <hyperlink ref="D7" r:id="rId25" display="https://bitbucket.org/zhufine/iosapp/downloads/pesoq-pro-1.0.2-2-prod.ipa" tooltip="https://bitbucket.org/zhufine/iosapp/downloads/pesoq-pro-1.0.2-2-prod.ipa"/>
-    <hyperlink ref="D6" r:id="rId26" display="https://bitbucket.org/zhufine/iosapp/downloads/pesoq-pro-1.0.3-1-prod.ipa"/>
-    <hyperlink ref="D5" r:id="rId27" display="https://bitbucket.org/zhufine/iosapp/downloads/pesoq-pro-1.0.3-2-prod.ipa"/>
-    <hyperlink ref="D4" r:id="rId28" display="https://bitbucket.org/zhufine/iosapp/downloads/ipesovip-test-1.0.1-3.ipa"/>
-    <hyperlink ref="D3" r:id="rId29" display="https://bitbucket.org/zhufine/iosapp/downloads/ipesovip-1.0.1-4-test.ipa" tooltip="https://bitbucket.org/zhufine/iosapp/downloads/ipesovip-1.0.1-4-test.ipa"/>
-    <hyperlink ref="D2" r:id="rId30" display="https://bitbucket.org/zhufine/iosapp/downloads/ipesovip-1.0.2-1-test.ipa" tooltip="https://bitbucket.org/zhufine/iosapp/downloads/ipesovip-1.0.2-1-test.ipa"/>
+    <hyperlink ref="D32" r:id="rId1" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.2-3.ipa"/>
+    <hyperlink ref="D31" r:id="rId2" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.2-4.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.2-4.ipa"/>
+    <hyperlink ref="D30" r:id="rId3" display="https://bitbucket.org/cop-dev/ios-apps/downloads/Ipeso-1.0.1-test1.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/Ipeso-1.0.1-test1.ipa"/>
+    <hyperlink ref="D29" r:id="rId4" display="https://bitbucket.org/cop-dev/ios-apps/downloads/Ipeso-1.0.2-2-test.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/Ipeso-1.0.2-2-test.ipa"/>
+    <hyperlink ref="D28" r:id="rId5" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.3-2-test.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.3-2-test.ipa"/>
+    <hyperlink ref="D27" r:id="rId6" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.3-3-prod.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/pautangpeso-1.0.3-3-prod.ipa"/>
+    <hyperlink ref="D26" r:id="rId7" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pesoq-test-1.5.6-3.ipa"/>
+    <hyperlink ref="D25" r:id="rId8" display="https://bitbucket.org/cop-dev/ios-apps/downloads/pesocash-test-1.3.0-1.ipa"/>
+    <hyperlink ref="D24" r:id="rId9" display="https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.0-2.test.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.0-2.test.ipa"/>
+    <hyperlink ref="D23" r:id="rId10" display="https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.1-1-prod.ipa"/>
+    <hyperlink ref="D22" r:id="rId11" display="https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.2-1-test.ipa"/>
+    <hyperlink ref="D21" r:id="rId12" display="https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.2-1-prod.ipa" tooltip="https://bitbucket.org/cop-dev/ios-apps/downloads/cashwill-1.0.2-1-prod.ipa"/>
+    <hyperlink ref="D20" r:id="rId13" display="https://bitbucket.org/ios4/ios/downloads/pautangpeso-1.0.4-1-test.ipa"/>
+    <hyperlink ref="D19" r:id="rId14" display="https://bitbucket.org/ios4/ios/downloads/pesoq-1.5.6-3-prod.ipa" tooltip="https://bitbucket.org/ios4/ios/downloads/pesoq-1.5.6-3-prod.ipa"/>
+    <hyperlink ref="D18" r:id="rId15" display="https://bitbucket.org/ios4/ios/downloads/pautangpeso-1.0.4-1-prod.ipa"/>
+    <hyperlink ref="D17" r:id="rId16" display="https://bitbucket.org/ios4/ios/downloads/pesoq-1.5.6-3-test.ipa"/>
+    <hyperlink ref="D16" r:id="rId17" display="https://bitbucket.org/ios4/ios/downloads/pesoq-prod-1.5.7-1.ipa" tooltip="https://bitbucket.org/ios4/ios/downloads/pesoq-prod-1.5.7-1.ipa"/>
+    <hyperlink ref="D15" r:id="rId18" display="https://bitbucket.org/ios4/ios/downloads/ipesovip-test-1.0.1-1.ipa"/>
+    <hyperlink ref="D14" r:id="rId19" display="https://bitbucket.org/zhufine/iosfine/downloads/ipesovip-prod-1.0.1-2.ipa" tooltip="https://bitbucket.org/zhufine/iosfine/downloads/ipesovip-prod-1.0.1-2.ipa"/>
+    <hyperlink ref="D13" r:id="rId20" display="https://bitbucket.org/zhufine/iosfine/downloads/pesoq-pro-test-1.0.1-1.ipa" tooltip="https://bitbucket.org/zhufine/iosfine/downloads/pesoq-pro-test-1.0.1-1.ipa"/>
+    <hyperlink ref="D12" r:id="rId21" display="https://bitbucket.org/zhufine/iosfine/downloads/pesoq-pro-1.0.1-1-prod.ipa" tooltip="https://bitbucket.org/zhufine/iosfine/downloads/pesoq-pro-1.0.1-1-prod.ipa"/>
+    <hyperlink ref="D11" r:id="rId22" display="https://bitbucket.org/zhufine/iosfine/downloads/pesoq-pro-test-1.0.1-3.ipa"/>
+    <hyperlink ref="D9" r:id="rId23" display="https://bitbucket.org/zhufine/iosfine/downloads/pesoq-pro-1.0.2-1-test.ipa"/>
+    <hyperlink ref="D10" r:id="rId24" display="https://bitbucket.org/zhufine/iosfine/downloads/pesoq-pro-1.0.2-1-prod.ipa"/>
+    <hyperlink ref="D8" r:id="rId25" display="https://bitbucket.org/zhufine/iosapp/downloads/pesoq-pro-1.0.2-2-prod.ipa" tooltip="https://bitbucket.org/zhufine/iosapp/downloads/pesoq-pro-1.0.2-2-prod.ipa"/>
+    <hyperlink ref="D7" r:id="rId26" display="https://bitbucket.org/zhufine/iosapp/downloads/pesoq-pro-1.0.3-1-prod.ipa"/>
+    <hyperlink ref="D6" r:id="rId27" display="https://bitbucket.org/zhufine/iosapp/downloads/pesoq-pro-1.0.3-2-prod.ipa"/>
+    <hyperlink ref="D5" r:id="rId28" display="https://bitbucket.org/zhufine/iosapp/downloads/ipesovip-test-1.0.1-3.ipa"/>
+    <hyperlink ref="D4" r:id="rId29" display="https://bitbucket.org/zhufine/iosapp/downloads/ipesovip-1.0.1-4-test.ipa" tooltip="https://bitbucket.org/zhufine/iosapp/downloads/ipesovip-1.0.1-4-test.ipa"/>
+    <hyperlink ref="D3" r:id="rId30" display="https://bitbucket.org/zhufine/iosapp/downloads/ipesovip-1.0.2-1-test.ipa" tooltip="https://bitbucket.org/zhufine/iosapp/downloads/ipesovip-1.0.2-1-test.ipa"/>
+    <hyperlink ref="D2" r:id="rId31" display="https://bitbucket.org/zhufine/iosapp/downloads/ipesovip-1.0.2-1-prod.ipa"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>